<commit_message>
Alta de Rubros y Alta de Silos terminada
</commit_message>
<xml_diff>
--- a/datos TP3.xlsx
+++ b/datos TP3.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Public\ESTUDIO\AyED\TP3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HorusPC\Desktop\GIT-Test\tpn3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B95FE884-BF83-47EC-B3D2-91BBBD3E453E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{064B514C-F481-46D5-8CCD-2530D57268CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8EB02DBB-B152-41AD-9533-88013EE04A21}"/>
   </bookViews>
@@ -41,16 +41,16 @@
     <comment ref="M48" authorId="0" shapeId="0" xr:uid="{762ED5EC-C72C-4A18-A897-FD66AE10642D}">
       <text/>
     </comment>
-    <comment ref="M49" authorId="0" shapeId="0" xr:uid="{3E926ED2-AC54-4DD1-9E06-A2B266177BD9}">
+    <comment ref="M51" authorId="0" shapeId="0" xr:uid="{3E926ED2-AC54-4DD1-9E06-A2B266177BD9}">
       <text/>
     </comment>
-    <comment ref="M50" authorId="0" shapeId="0" xr:uid="{0B0F310E-15BC-40C0-BF0E-5ED516A21967}">
+    <comment ref="M54" authorId="0" shapeId="0" xr:uid="{0B0F310E-15BC-40C0-BF0E-5ED516A21967}">
       <text/>
     </comment>
-    <comment ref="M51" authorId="0" shapeId="0" xr:uid="{28FC0ADB-A958-48F2-930D-9AA4E5F0E5BF}">
+    <comment ref="M57" authorId="0" shapeId="0" xr:uid="{28FC0ADB-A958-48F2-930D-9AA4E5F0E5BF}">
       <text/>
     </comment>
-    <comment ref="M52" authorId="0" shapeId="0" xr:uid="{F2504DD1-B37A-402F-B3D8-DA8C028C09CD}">
+    <comment ref="M60" authorId="0" shapeId="0" xr:uid="{F2504DD1-B37A-402F-B3D8-DA8C028C09CD}">
       <text/>
     </comment>
   </commentList>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="76">
   <si>
     <t>productos</t>
   </si>
@@ -261,15 +261,6 @@
     <t>PUNTA NEGRA CARBON</t>
   </si>
   <si>
-    <t>RUBRO 1</t>
-  </si>
-  <si>
-    <t>RUBRO 2</t>
-  </si>
-  <si>
-    <t>RUBRO 3</t>
-  </si>
-  <si>
     <t>SILOS.DAT</t>
   </si>
   <si>
@@ -286,6 +277,15 @@
   </si>
   <si>
     <t>n</t>
+  </si>
+  <si>
+    <t>COD RUB</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
   </si>
 </sst>
 </file>
@@ -606,11 +606,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -731,6 +731,50 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>410099</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>181329</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8DFE2DD-CD59-E635-21D6-11ABCA9917F7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13487400" y="6286500"/>
+          <a:ext cx="3753374" cy="2534004"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1033,10 +1077,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F70E36C0-A77A-46FF-BE02-DF3DE3726FE3}">
-  <dimension ref="A1:R61"/>
+  <dimension ref="A1:R71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="L60" sqref="L60"/>
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1089,17 +1133,17 @@
       <c r="B3" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="33" t="s">
+      <c r="D3" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
       <c r="G3" s="2"/>
-      <c r="I3" s="33" t="s">
+      <c r="I3" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
     </row>
     <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
@@ -1384,14 +1428,14 @@
       <c r="I15" t="s">
         <v>28</v>
       </c>
-      <c r="K15" s="34"/>
-      <c r="L15" s="34"/>
-      <c r="M15" s="34"/>
-      <c r="N15" s="34"/>
-      <c r="O15" s="34"/>
-      <c r="P15" s="34"/>
-      <c r="Q15" s="34"/>
-      <c r="R15" s="34"/>
+      <c r="K15" s="33"/>
+      <c r="L15" s="33"/>
+      <c r="M15" s="33"/>
+      <c r="N15" s="33"/>
+      <c r="O15" s="33"/>
+      <c r="P15" s="33"/>
+      <c r="Q15" s="33"/>
+      <c r="R15" s="33"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
@@ -1418,7 +1462,7 @@
       <c r="J16" s="4">
         <v>1</v>
       </c>
-      <c r="K16" s="34"/>
+      <c r="K16" s="33"/>
       <c r="N16" t="s">
         <v>51</v>
       </c>
@@ -1448,7 +1492,7 @@
       <c r="J17" t="s">
         <v>30</v>
       </c>
-      <c r="K17" s="34"/>
+      <c r="K17" s="33"/>
       <c r="L17" s="8" t="s">
         <v>50</v>
       </c>
@@ -1470,7 +1514,7 @@
       </c>
       <c r="I18" s="22"/>
       <c r="J18" s="23"/>
-      <c r="K18" s="34"/>
+      <c r="K18" s="33"/>
       <c r="L18" s="4"/>
       <c r="M18" s="4" t="s">
         <v>52</v>
@@ -1492,7 +1536,7 @@
       </c>
       <c r="I19" s="24"/>
       <c r="J19" s="25"/>
-      <c r="K19" s="34"/>
+      <c r="K19" s="33"/>
       <c r="L19">
         <v>0</v>
       </c>
@@ -1513,7 +1557,7 @@
       </c>
       <c r="I20" s="26"/>
       <c r="J20" s="27"/>
-      <c r="K20" s="34"/>
+      <c r="K20" s="33"/>
       <c r="L20">
         <v>1</v>
       </c>
@@ -1522,7 +1566,7 @@
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="K21" s="34"/>
+      <c r="K21" s="33"/>
       <c r="L21">
         <v>2</v>
       </c>
@@ -1531,7 +1575,7 @@
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="K22" s="34"/>
+      <c r="K22" s="33"/>
       <c r="L22">
         <v>3</v>
       </c>
@@ -1546,7 +1590,7 @@
       <c r="B23" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="K23" s="34"/>
+      <c r="K23" s="33"/>
       <c r="L23">
         <v>4</v>
       </c>
@@ -1558,7 +1602,7 @@
       <c r="A24" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="K24" s="34"/>
+      <c r="K24" s="33"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
@@ -1567,7 +1611,7 @@
       <c r="B25" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="K25" s="34"/>
+      <c r="K25" s="33"/>
       <c r="L25" s="8" t="s">
         <v>50</v>
       </c>
@@ -1587,7 +1631,7 @@
       <c r="B26" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="K26" s="34"/>
+      <c r="K26" s="33"/>
       <c r="L26" s="4"/>
       <c r="M26" s="4" t="s">
         <v>38</v>
@@ -1615,7 +1659,7 @@
       <c r="B27" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="K27" s="34"/>
+      <c r="K27" s="33"/>
       <c r="L27">
         <v>0</v>
       </c>
@@ -1627,7 +1671,7 @@
       <c r="B28" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="K28" s="34"/>
+      <c r="K28" s="33"/>
       <c r="L28">
         <v>1</v>
       </c>
@@ -1639,38 +1683,38 @@
       <c r="B29" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="K29" s="34"/>
+      <c r="K29" s="33"/>
       <c r="L29">
         <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="K30" s="34"/>
+      <c r="K30" s="33"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="K31" s="34"/>
+      <c r="K31" s="33"/>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="K32" s="34"/>
+      <c r="K32" s="33"/>
       <c r="L32" s="8"/>
       <c r="M32" s="8" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="33" spans="11:17" x14ac:dyDescent="0.25">
-      <c r="K33" s="34"/>
+      <c r="K33" s="33"/>
       <c r="L33" s="4" t="s">
         <v>50</v>
       </c>
       <c r="M33" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="N33" s="35" t="s">
-        <v>74</v>
+      <c r="N33" s="34" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="11:17" x14ac:dyDescent="0.25">
-      <c r="K34" s="34"/>
+      <c r="K34" s="33"/>
       <c r="L34">
         <v>0</v>
       </c>
@@ -1679,7 +1723,7 @@
       </c>
     </row>
     <row r="35" spans="11:17" x14ac:dyDescent="0.25">
-      <c r="K35" s="34"/>
+      <c r="K35" s="33"/>
       <c r="L35">
         <v>1</v>
       </c>
@@ -1688,7 +1732,7 @@
       </c>
     </row>
     <row r="36" spans="11:17" x14ac:dyDescent="0.25">
-      <c r="K36" s="34"/>
+      <c r="K36" s="33"/>
       <c r="L36">
         <v>2</v>
       </c>
@@ -1697,7 +1741,7 @@
       </c>
     </row>
     <row r="37" spans="11:17" x14ac:dyDescent="0.25">
-      <c r="K37" s="34"/>
+      <c r="K37" s="33"/>
       <c r="L37">
         <v>3</v>
       </c>
@@ -1706,7 +1750,7 @@
       </c>
     </row>
     <row r="38" spans="11:17" x14ac:dyDescent="0.25">
-      <c r="K38" s="34"/>
+      <c r="K38" s="33"/>
       <c r="L38">
         <v>4</v>
       </c>
@@ -1715,7 +1759,7 @@
       </c>
     </row>
     <row r="39" spans="11:17" x14ac:dyDescent="0.25">
-      <c r="K39" s="34"/>
+      <c r="K39" s="33"/>
       <c r="L39">
         <v>5</v>
       </c>
@@ -1724,7 +1768,7 @@
       </c>
     </row>
     <row r="40" spans="11:17" x14ac:dyDescent="0.25">
-      <c r="K40" s="34"/>
+      <c r="K40" s="33"/>
       <c r="L40">
         <v>6</v>
       </c>
@@ -1733,7 +1777,7 @@
       </c>
     </row>
     <row r="41" spans="11:17" x14ac:dyDescent="0.25">
-      <c r="K41" s="34"/>
+      <c r="K41" s="33"/>
       <c r="L41">
         <v>7</v>
       </c>
@@ -1742,7 +1786,7 @@
       </c>
     </row>
     <row r="42" spans="11:17" x14ac:dyDescent="0.25">
-      <c r="K42" s="34"/>
+      <c r="K42" s="33"/>
       <c r="L42">
         <v>8</v>
       </c>
@@ -1751,7 +1795,7 @@
       </c>
     </row>
     <row r="43" spans="11:17" x14ac:dyDescent="0.25">
-      <c r="K43" s="34"/>
+      <c r="K43" s="33"/>
       <c r="L43">
         <v>9</v>
       </c>
@@ -1760,7 +1804,7 @@
       </c>
     </row>
     <row r="44" spans="11:17" x14ac:dyDescent="0.25">
-      <c r="K44" s="34"/>
+      <c r="K44" s="33"/>
       <c r="L44">
         <v>10</v>
       </c>
@@ -1769,10 +1813,10 @@
       </c>
     </row>
     <row r="45" spans="11:17" x14ac:dyDescent="0.25">
-      <c r="K45" s="34"/>
+      <c r="K45" s="33"/>
     </row>
     <row r="46" spans="11:17" x14ac:dyDescent="0.25">
-      <c r="K46" s="34"/>
+      <c r="K46" s="33"/>
       <c r="L46" s="8"/>
       <c r="M46" s="8" t="s">
         <v>54</v>
@@ -1783,157 +1827,233 @@
       <c r="Q46" s="8"/>
     </row>
     <row r="47" spans="11:17" x14ac:dyDescent="0.25">
-      <c r="K47" s="34"/>
+      <c r="K47" s="33"/>
       <c r="L47" s="4"/>
-      <c r="M47" s="4" t="s">
+      <c r="M47" s="4"/>
+      <c r="N47" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="N47" s="4" t="s">
-        <v>55</v>
-      </c>
       <c r="O47" s="4" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="P47" s="4" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="Q47" s="4" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
     </row>
     <row r="48" spans="11:17" x14ac:dyDescent="0.25">
-      <c r="K48" s="34"/>
+      <c r="K48" s="33"/>
       <c r="L48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M48" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="49" spans="11:17" x14ac:dyDescent="0.25">
-      <c r="K49" s="34"/>
+      <c r="N48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K49" s="33"/>
       <c r="L49">
         <v>1</v>
       </c>
-      <c r="M49" t="s">
+      <c r="N49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K50" s="33"/>
+      <c r="L50">
+        <v>1</v>
+      </c>
+      <c r="N50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K51" s="33"/>
+      <c r="L51">
+        <v>2</v>
+      </c>
+      <c r="M51" t="s">
         <v>46</v>
       </c>
-      <c r="O49">
-        <v>10</v>
-      </c>
-      <c r="P49">
+      <c r="N51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K52" s="33"/>
+      <c r="L52">
+        <v>2</v>
+      </c>
+      <c r="N52">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K53" s="33"/>
+      <c r="L53">
+        <v>2</v>
+      </c>
+      <c r="N53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K54" s="33"/>
+      <c r="L54">
+        <v>3</v>
+      </c>
+      <c r="M54" t="s">
+        <v>47</v>
+      </c>
+      <c r="N54">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K55" s="33"/>
+      <c r="L55">
+        <v>3</v>
+      </c>
+      <c r="N55">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K56" s="33"/>
+      <c r="L56">
+        <v>3</v>
+      </c>
+      <c r="N56">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K57" s="33"/>
+      <c r="L57">
+        <v>4</v>
+      </c>
+      <c r="M57" t="s">
+        <v>48</v>
+      </c>
+      <c r="N57">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K58" s="33"/>
+      <c r="L58">
+        <v>4</v>
+      </c>
+      <c r="N58">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K59" s="33"/>
+      <c r="L59">
+        <v>4</v>
+      </c>
+      <c r="N59">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K60" s="33"/>
+      <c r="L60">
+        <v>5</v>
+      </c>
+      <c r="M60" t="s">
+        <v>49</v>
+      </c>
+      <c r="N60">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K61" s="33"/>
+      <c r="L61">
+        <v>5</v>
+      </c>
+      <c r="N61">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K62" s="33"/>
+      <c r="L62">
+        <v>5</v>
+      </c>
+      <c r="N62">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K63" s="33"/>
+    </row>
+    <row r="64" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K64" s="33"/>
+      <c r="L64" s="8"/>
+      <c r="M64" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="N64" s="8"/>
+      <c r="O64" s="8"/>
+      <c r="P64" s="8"/>
+    </row>
+    <row r="65" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K65" s="33"/>
+      <c r="L65" s="4"/>
+      <c r="M65" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="N65" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="O65" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="P65" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="66" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K66" s="33"/>
+      <c r="L66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K67" s="33"/>
+      <c r="L67">
         <v>1</v>
       </c>
-      <c r="Q49">
+    </row>
+    <row r="68" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K68" s="33"/>
+      <c r="L68">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K69" s="33"/>
+      <c r="L69">
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="11:17" x14ac:dyDescent="0.25">
-      <c r="K50" s="34"/>
-      <c r="L50">
-        <v>2</v>
-      </c>
-      <c r="M50" t="s">
-        <v>47</v>
-      </c>
-      <c r="O50">
-        <v>1</v>
-      </c>
-      <c r="P50">
-        <v>2</v>
-      </c>
-      <c r="Q50">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="51" spans="11:17" x14ac:dyDescent="0.25">
-      <c r="K51" s="34"/>
-      <c r="L51">
-        <v>3</v>
-      </c>
-      <c r="M51" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="52" spans="11:17" x14ac:dyDescent="0.25">
-      <c r="K52" s="34"/>
-      <c r="L52">
-        <v>4</v>
-      </c>
-      <c r="M52" t="s">
-        <v>49</v>
-      </c>
-      <c r="O52">
-        <v>1</v>
-      </c>
-      <c r="P52">
-        <v>4</v>
-      </c>
-      <c r="Q52">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="53" spans="11:17" x14ac:dyDescent="0.25">
-      <c r="K53" s="34"/>
-    </row>
-    <row r="54" spans="11:17" x14ac:dyDescent="0.25">
-      <c r="K54" s="34"/>
-      <c r="L54" s="8"/>
-      <c r="M54" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="N54" s="8"/>
-      <c r="O54" s="8"/>
-      <c r="P54" s="8"/>
-    </row>
-    <row r="55" spans="11:17" x14ac:dyDescent="0.25">
-      <c r="K55" s="34"/>
-      <c r="L55" s="4"/>
-      <c r="M55" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="N55" s="4" t="s">
+    <row r="70" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K70" s="33"/>
+      <c r="L70" t="s">
         <v>72</v>
       </c>
-      <c r="O55" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="P55" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="56" spans="11:17" x14ac:dyDescent="0.25">
-      <c r="K56" s="34"/>
-      <c r="L56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="11:17" x14ac:dyDescent="0.25">
-      <c r="K57" s="34"/>
-      <c r="L57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="11:17" x14ac:dyDescent="0.25">
-      <c r="K58" s="34"/>
-      <c r="L58">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="59" spans="11:17" x14ac:dyDescent="0.25">
-      <c r="K59" s="34"/>
-      <c r="L59">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="60" spans="11:17" x14ac:dyDescent="0.25">
-      <c r="K60" s="34"/>
-      <c r="L60" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="61" spans="11:17" x14ac:dyDescent="0.25">
-      <c r="K61" s="34"/>
+    </row>
+    <row r="71" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K71" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
BRUTO Y TARA EN modificación. CUPOS, NUEVA VERSION.
</commit_message>
<xml_diff>
--- a/datos TP3.xlsx
+++ b/datos TP3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HorusPC\Desktop\GIT-Test\tpn3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{064B514C-F481-46D5-8CCD-2530D57268CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CADB2347-C79B-4468-A22E-036C0175594E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8EB02DBB-B152-41AD-9533-88013EE04A21}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="87">
   <si>
     <t>productos</t>
   </si>
@@ -286,6 +286,39 @@
   </si>
   <si>
     <t>max</t>
+  </si>
+  <si>
+    <t>50-60</t>
+  </si>
+  <si>
+    <t>ilegal</t>
+  </si>
+  <si>
+    <t>lega</t>
+  </si>
+  <si>
+    <t>ejes</t>
+  </si>
+  <si>
+    <t>simple</t>
+  </si>
+  <si>
+    <t xml:space="preserve">doble </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tandem </t>
+  </si>
+  <si>
+    <t>triple</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rueda </t>
+  </si>
+  <si>
+    <t>direccional</t>
+  </si>
+  <si>
+    <t>peso cami</t>
   </si>
 </sst>
 </file>
@@ -1079,8 +1112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F70E36C0-A77A-46FF-BE02-DF3DE3726FE3}">
   <dimension ref="A1:R71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="F55" sqref="F55"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1701,7 +1734,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="11:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:17" x14ac:dyDescent="0.25">
       <c r="K33" s="33"/>
       <c r="L33" s="4" t="s">
         <v>50</v>
@@ -1713,7 +1746,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="34" spans="11:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:17" x14ac:dyDescent="0.25">
       <c r="K34" s="33"/>
       <c r="L34">
         <v>0</v>
@@ -1722,7 +1755,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="11:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:17" x14ac:dyDescent="0.25">
       <c r="K35" s="33"/>
       <c r="L35">
         <v>1</v>
@@ -1731,7 +1764,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="11:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:17" x14ac:dyDescent="0.25">
       <c r="K36" s="33"/>
       <c r="L36">
         <v>2</v>
@@ -1740,7 +1773,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="37" spans="11:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:17" x14ac:dyDescent="0.25">
       <c r="K37" s="33"/>
       <c r="L37">
         <v>3</v>
@@ -1749,7 +1782,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="38" spans="11:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:17" x14ac:dyDescent="0.25">
       <c r="K38" s="33"/>
       <c r="L38">
         <v>4</v>
@@ -1758,7 +1791,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="39" spans="11:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:17" x14ac:dyDescent="0.25">
       <c r="K39" s="33"/>
       <c r="L39">
         <v>5</v>
@@ -1767,7 +1800,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="40" spans="11:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:17" x14ac:dyDescent="0.25">
       <c r="K40" s="33"/>
       <c r="L40">
         <v>6</v>
@@ -1776,7 +1809,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="41" spans="11:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:17" x14ac:dyDescent="0.25">
       <c r="K41" s="33"/>
       <c r="L41">
         <v>7</v>
@@ -1785,7 +1818,13 @@
         <v>62</v>
       </c>
     </row>
-    <row r="42" spans="11:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="E42" t="s">
+        <v>77</v>
+      </c>
+      <c r="F42" t="s">
+        <v>76</v>
+      </c>
       <c r="K42" s="33"/>
       <c r="L42">
         <v>8</v>
@@ -1794,7 +1833,13 @@
         <v>63</v>
       </c>
     </row>
-    <row r="43" spans="11:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="E43" t="s">
+        <v>78</v>
+      </c>
+      <c r="F43">
+        <v>45</v>
+      </c>
       <c r="K43" s="33"/>
       <c r="L43">
         <v>9</v>
@@ -1803,7 +1848,13 @@
         <v>65</v>
       </c>
     </row>
-    <row r="44" spans="11:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="E44" t="s">
+        <v>6</v>
+      </c>
+      <c r="F44">
+        <v>30</v>
+      </c>
       <c r="K44" s="33"/>
       <c r="L44">
         <v>10</v>
@@ -1812,10 +1863,22 @@
         <v>66</v>
       </c>
     </row>
-    <row r="45" spans="11:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
+        <v>86</v>
+      </c>
+      <c r="E45">
+        <v>8</v>
+      </c>
+      <c r="F45">
+        <v>15</v>
+      </c>
       <c r="K45" s="33"/>
     </row>
-    <row r="46" spans="11:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="E46" t="s">
+        <v>79</v>
+      </c>
       <c r="K46" s="33"/>
       <c r="L46" s="8"/>
       <c r="M46" s="8" t="s">
@@ -1826,7 +1889,13 @@
       <c r="P46" s="8"/>
       <c r="Q46" s="8"/>
     </row>
-    <row r="47" spans="11:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="E47" t="s">
+        <v>80</v>
+      </c>
+      <c r="F47">
+        <v>10.5</v>
+      </c>
       <c r="K47" s="33"/>
       <c r="L47" s="4"/>
       <c r="M47" s="4"/>
@@ -1843,7 +1912,16 @@
         <v>75</v>
       </c>
     </row>
-    <row r="48" spans="11:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D48" t="s">
+        <v>82</v>
+      </c>
+      <c r="E48" t="s">
+        <v>81</v>
+      </c>
+      <c r="F48">
+        <v>18</v>
+      </c>
       <c r="K48" s="33"/>
       <c r="L48">
         <v>1</v>
@@ -1854,8 +1932,17 @@
       <c r="N48">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="O48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="E49" t="s">
+        <v>83</v>
+      </c>
+      <c r="F49">
+        <v>25</v>
+      </c>
       <c r="K49" s="33"/>
       <c r="L49">
         <v>1</v>
@@ -1863,8 +1950,20 @@
       <c r="N49">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="O49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D50" t="s">
+        <v>84</v>
+      </c>
+      <c r="E50" t="s">
+        <v>85</v>
+      </c>
+      <c r="F50">
+        <v>6</v>
+      </c>
       <c r="K50" s="33"/>
       <c r="L50">
         <v>1</v>
@@ -1872,8 +1971,11 @@
       <c r="N50">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="O50">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="4:16" x14ac:dyDescent="0.25">
       <c r="K51" s="33"/>
       <c r="L51">
         <v>2</v>
@@ -1884,8 +1986,11 @@
       <c r="N51">
         <v>2</v>
       </c>
-    </row>
-    <row r="52" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="O51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="4:16" x14ac:dyDescent="0.25">
       <c r="K52" s="33"/>
       <c r="L52">
         <v>2</v>
@@ -1893,8 +1998,11 @@
       <c r="N52">
         <v>2</v>
       </c>
-    </row>
-    <row r="53" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="O52">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="4:16" x14ac:dyDescent="0.25">
       <c r="K53" s="33"/>
       <c r="L53">
         <v>2</v>
@@ -1902,8 +2010,11 @@
       <c r="N53">
         <v>2</v>
       </c>
-    </row>
-    <row r="54" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="O53">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="4:16" x14ac:dyDescent="0.25">
       <c r="K54" s="33"/>
       <c r="L54">
         <v>3</v>
@@ -1914,8 +2025,11 @@
       <c r="N54">
         <v>3</v>
       </c>
-    </row>
-    <row r="55" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="O54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="4:16" x14ac:dyDescent="0.25">
       <c r="K55" s="33"/>
       <c r="L55">
         <v>3</v>
@@ -1923,8 +2037,11 @@
       <c r="N55">
         <v>3</v>
       </c>
-    </row>
-    <row r="56" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="O55">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="4:16" x14ac:dyDescent="0.25">
       <c r="K56" s="33"/>
       <c r="L56">
         <v>3</v>
@@ -1932,8 +2049,11 @@
       <c r="N56">
         <v>3</v>
       </c>
-    </row>
-    <row r="57" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="O56">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57" spans="4:16" x14ac:dyDescent="0.25">
       <c r="K57" s="33"/>
       <c r="L57">
         <v>4</v>
@@ -1944,8 +2064,11 @@
       <c r="N57">
         <v>4</v>
       </c>
-    </row>
-    <row r="58" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="O57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="4:16" x14ac:dyDescent="0.25">
       <c r="K58" s="33"/>
       <c r="L58">
         <v>4</v>
@@ -1953,8 +2076,11 @@
       <c r="N58">
         <v>4</v>
       </c>
-    </row>
-    <row r="59" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="O58">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="4:16" x14ac:dyDescent="0.25">
       <c r="K59" s="33"/>
       <c r="L59">
         <v>4</v>
@@ -1962,8 +2088,11 @@
       <c r="N59">
         <v>4</v>
       </c>
-    </row>
-    <row r="60" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="O59">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="4:16" x14ac:dyDescent="0.25">
       <c r="K60" s="33"/>
       <c r="L60">
         <v>5</v>
@@ -1974,8 +2103,11 @@
       <c r="N60">
         <v>5</v>
       </c>
-    </row>
-    <row r="61" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="O60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="4:16" x14ac:dyDescent="0.25">
       <c r="K61" s="33"/>
       <c r="L61">
         <v>5</v>
@@ -1983,8 +2115,11 @@
       <c r="N61">
         <v>5</v>
       </c>
-    </row>
-    <row r="62" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="O61">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="4:16" x14ac:dyDescent="0.25">
       <c r="K62" s="33"/>
       <c r="L62">
         <v>5</v>
@@ -1992,11 +2127,14 @@
       <c r="N62">
         <v>5</v>
       </c>
-    </row>
-    <row r="63" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="O62">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="4:16" x14ac:dyDescent="0.25">
       <c r="K63" s="33"/>
     </row>
-    <row r="64" spans="11:16" x14ac:dyDescent="0.25">
+    <row r="64" spans="4:16" x14ac:dyDescent="0.25">
       <c r="K64" s="33"/>
       <c r="L64" s="8"/>
       <c r="M64" s="8" t="s">

</xml_diff>

<commit_message>
OK, ya funciona todo hasta el 6
</commit_message>
<xml_diff>
--- a/datos TP3.xlsx
+++ b/datos TP3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HorusPC\Desktop\GIT-Test\tpn3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CADB2347-C79B-4468-A22E-036C0175594E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D64F577D-71C4-45AA-8320-AFD16649C908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8EB02DBB-B152-41AD-9533-88013EE04A21}"/>
+    <workbookView xWindow="7005" yWindow="4170" windowWidth="2775" windowHeight="900" xr2:uid="{8EB02DBB-B152-41AD-9533-88013EE04A21}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="121">
   <si>
     <t>productos</t>
   </si>
@@ -319,6 +319,108 @@
   </si>
   <si>
     <t>peso cami</t>
+  </si>
+  <si>
+    <t>Maiz:</t>
+  </si>
+  <si>
+    <t>Ph:75kg/hl(mínimo)</t>
+  </si>
+  <si>
+    <t>Humedad:14,5%(máximo)</t>
+  </si>
+  <si>
+    <t>Granos picados:3,00%(máximo)</t>
+  </si>
+  <si>
+    <t>Sorgo granifero:</t>
+  </si>
+  <si>
+    <t>Humedad:15%(máximo)</t>
+  </si>
+  <si>
+    <t>Granos dañados:2%(máximo)</t>
+  </si>
+  <si>
+    <t>Trigo forrajero:</t>
+  </si>
+  <si>
+    <t>Ph mínimo: 72,6kg/hl (mínimo)</t>
+  </si>
+  <si>
+    <t>Humedad:14%(máximo)</t>
+  </si>
+  <si>
+    <t>Insectos:nada,o%</t>
+  </si>
+  <si>
+    <t>Cebada cervecera:</t>
+  </si>
+  <si>
+    <t>Humedad:12,5%(máximo)</t>
+  </si>
+  <si>
+    <t>Proteína mínima:9,5%</t>
+  </si>
+  <si>
+    <t>Proteína máxima:13%</t>
+  </si>
+  <si>
+    <t>Girasol:</t>
+  </si>
+  <si>
+    <t>Humedad:14,0% (máxima)</t>
+  </si>
+  <si>
+    <t>Materias grasas:no entiendo la cifra</t>
+  </si>
+  <si>
+    <t>Materias extrañas:3,0% (máximo)</t>
+  </si>
+  <si>
+    <t>Alpiste:</t>
+  </si>
+  <si>
+    <t>Chamico:2 semillas c/100gr</t>
+  </si>
+  <si>
+    <t>Humedad:14% (máximo)</t>
+  </si>
+  <si>
+    <t>Cornezuelo:0,1%(máximo)</t>
+  </si>
+  <si>
+    <t>Avena:</t>
+  </si>
+  <si>
+    <t>Ph mínimo:46 /Kg</t>
+  </si>
+  <si>
+    <t>Granos manchados: ligeramente</t>
+  </si>
+  <si>
+    <t>Humedad: 14%(máximo)</t>
+  </si>
+  <si>
+    <t>Mijo:</t>
+  </si>
+  <si>
+    <t>Picado:10%(máximo)</t>
+  </si>
+  <si>
+    <t>Granos dañados:0,50%(máximo)</t>
+  </si>
+  <si>
+    <t>Centeno:</t>
+  </si>
+  <si>
+    <t>Ph mínimo:70/Kg</t>
+  </si>
+  <si>
+    <t>Cornezuelo:0,05%(máximo)</t>
+  </si>
+  <si>
+    <t>Tolerancia de picado:1,0%(máximo)</t>
   </si>
 </sst>
 </file>
@@ -1110,10 +1212,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F70E36C0-A77A-46FF-BE02-DF3DE3726FE3}">
-  <dimension ref="A1:R71"/>
+  <dimension ref="A1:R83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" topLeftCell="E31" workbookViewId="0">
+      <selection activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1810,6 +1912,9 @@
       </c>
     </row>
     <row r="41" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="H41" t="s">
+        <v>87</v>
+      </c>
       <c r="K41" s="33"/>
       <c r="L41">
         <v>7</v>
@@ -1825,6 +1930,9 @@
       <c r="F42" t="s">
         <v>76</v>
       </c>
+      <c r="H42" t="s">
+        <v>88</v>
+      </c>
       <c r="K42" s="33"/>
       <c r="L42">
         <v>8</v>
@@ -1840,6 +1948,9 @@
       <c r="F43">
         <v>45</v>
       </c>
+      <c r="H43" t="s">
+        <v>89</v>
+      </c>
       <c r="K43" s="33"/>
       <c r="L43">
         <v>9</v>
@@ -1855,6 +1966,9 @@
       <c r="F44">
         <v>30</v>
       </c>
+      <c r="H44" t="s">
+        <v>90</v>
+      </c>
       <c r="K44" s="33"/>
       <c r="L44">
         <v>10</v>
@@ -1878,6 +1992,9 @@
     <row r="46" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E46" t="s">
         <v>79</v>
+      </c>
+      <c r="H46" t="s">
+        <v>91</v>
       </c>
       <c r="K46" s="33"/>
       <c r="L46" s="8"/>
@@ -1895,6 +2012,9 @@
       </c>
       <c r="F47">
         <v>10.5</v>
+      </c>
+      <c r="H47" t="s">
+        <v>92</v>
       </c>
       <c r="K47" s="33"/>
       <c r="L47" s="4"/>
@@ -1922,6 +2042,9 @@
       <c r="F48">
         <v>18</v>
       </c>
+      <c r="H48" t="s">
+        <v>93</v>
+      </c>
       <c r="K48" s="33"/>
       <c r="L48">
         <v>1</v>
@@ -1964,6 +2087,9 @@
       <c r="F50">
         <v>6</v>
       </c>
+      <c r="H50" t="s">
+        <v>94</v>
+      </c>
       <c r="K50" s="33"/>
       <c r="L50">
         <v>1</v>
@@ -1976,6 +2102,9 @@
       </c>
     </row>
     <row r="51" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="H51" t="s">
+        <v>95</v>
+      </c>
       <c r="K51" s="33"/>
       <c r="L51">
         <v>2</v>
@@ -1991,6 +2120,9 @@
       </c>
     </row>
     <row r="52" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="H52" t="s">
+        <v>96</v>
+      </c>
       <c r="K52" s="33"/>
       <c r="L52">
         <v>2</v>
@@ -2003,6 +2135,9 @@
       </c>
     </row>
     <row r="53" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="H53" t="s">
+        <v>97</v>
+      </c>
       <c r="K53" s="33"/>
       <c r="L53">
         <v>2</v>
@@ -2030,6 +2165,9 @@
       </c>
     </row>
     <row r="55" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="H55" t="s">
+        <v>98</v>
+      </c>
       <c r="K55" s="33"/>
       <c r="L55">
         <v>3</v>
@@ -2042,6 +2180,9 @@
       </c>
     </row>
     <row r="56" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="H56" t="s">
+        <v>99</v>
+      </c>
       <c r="K56" s="33"/>
       <c r="L56">
         <v>3</v>
@@ -2054,6 +2195,9 @@
       </c>
     </row>
     <row r="57" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="H57" t="s">
+        <v>100</v>
+      </c>
       <c r="K57" s="33"/>
       <c r="L57">
         <v>4</v>
@@ -2069,6 +2213,9 @@
       </c>
     </row>
     <row r="58" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="H58" t="s">
+        <v>101</v>
+      </c>
       <c r="K58" s="33"/>
       <c r="L58">
         <v>4</v>
@@ -2093,6 +2240,9 @@
       </c>
     </row>
     <row r="60" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="H60" t="s">
+        <v>102</v>
+      </c>
       <c r="K60" s="33"/>
       <c r="L60">
         <v>5</v>
@@ -2108,6 +2258,9 @@
       </c>
     </row>
     <row r="61" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="H61" t="s">
+        <v>103</v>
+      </c>
       <c r="K61" s="33"/>
       <c r="L61">
         <v>5</v>
@@ -2120,6 +2273,9 @@
       </c>
     </row>
     <row r="62" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="H62" t="s">
+        <v>104</v>
+      </c>
       <c r="K62" s="33"/>
       <c r="L62">
         <v>5</v>
@@ -2132,6 +2288,9 @@
       </c>
     </row>
     <row r="63" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="H63" t="s">
+        <v>105</v>
+      </c>
       <c r="K63" s="33"/>
     </row>
     <row r="64" spans="4:16" x14ac:dyDescent="0.25">
@@ -2144,7 +2303,10 @@
       <c r="O64" s="8"/>
       <c r="P64" s="8"/>
     </row>
-    <row r="65" spans="11:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="H65" t="s">
+        <v>106</v>
+      </c>
       <c r="K65" s="33"/>
       <c r="L65" s="4"/>
       <c r="M65" s="4" t="s">
@@ -2160,38 +2322,103 @@
         <v>70</v>
       </c>
     </row>
-    <row r="66" spans="11:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="H66" t="s">
+        <v>107</v>
+      </c>
       <c r="K66" s="33"/>
       <c r="L66">
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="11:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="H67" t="s">
+        <v>108</v>
+      </c>
       <c r="K67" s="33"/>
       <c r="L67">
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="11:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="H68" t="s">
+        <v>109</v>
+      </c>
       <c r="K68" s="33"/>
       <c r="L68">
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="11:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="8:16" x14ac:dyDescent="0.25">
       <c r="K69" s="33"/>
       <c r="L69">
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="11:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="H70" t="s">
+        <v>110</v>
+      </c>
       <c r="K70" s="33"/>
       <c r="L70" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="71" spans="11:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="H71" t="s">
+        <v>111</v>
+      </c>
       <c r="K71" s="33"/>
+    </row>
+    <row r="72" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="H72" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="73" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="H73" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="75" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="H75" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="76" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="H76" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="77" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="H77" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="78" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="H78" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="80" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="H80" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="81" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H81" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="82" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H82" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="83" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H83" t="s">
+        <v>120</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Se agregó BRUTO y TARA. Y algunos Reportes.
</commit_message>
<xml_diff>
--- a/datos TP3.xlsx
+++ b/datos TP3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HorusPC\Desktop\GIT-Test\tpn3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D64F577D-71C4-45AA-8320-AFD16649C908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D69AC0-8743-45DD-B9DB-70BC41DE728E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7005" yWindow="4170" windowWidth="2775" windowHeight="900" xr2:uid="{8EB02DBB-B152-41AD-9533-88013EE04A21}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8EB02DBB-B152-41AD-9533-88013EE04A21}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="125">
   <si>
     <t>productos</t>
   </si>
@@ -421,6 +421,18 @@
   </si>
   <si>
     <t>Tolerancia de picado:1,0%(máximo)</t>
+  </si>
+  <si>
+    <t>Soja:</t>
+  </si>
+  <si>
+    <t>Granos Dañanos</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Max</t>
   </si>
 </sst>
 </file>
@@ -1212,10 +1224,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F70E36C0-A77A-46FF-BE02-DF3DE3726FE3}">
-  <dimension ref="A1:R83"/>
+  <dimension ref="A1:R88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E31" workbookViewId="0">
-      <selection activeCell="F59" sqref="F59"/>
+    <sheetView tabSelected="1" topLeftCell="E17" workbookViewId="0">
+      <selection activeCell="I88" sqref="H41:I88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2405,19 +2417,45 @@
         <v>117</v>
       </c>
     </row>
-    <row r="81" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H81" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="82" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H82" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="83" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H83" t="s">
         <v>120</v>
+      </c>
+    </row>
+    <row r="85" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H85" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="86" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H86" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="87" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H87" t="s">
+        <v>123</v>
+      </c>
+      <c r="I87">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="88" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H88" t="s">
+        <v>124</v>
+      </c>
+      <c r="I88">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ya casi terminando, estoy trabajando sobre la entrega de cupos y Rubros x Producto
</commit_message>
<xml_diff>
--- a/datos TP3.xlsx
+++ b/datos TP3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HorusPC\Desktop\GIT-Test\tpn3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D69AC0-8743-45DD-B9DB-70BC41DE728E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AFAAB51-C3B4-46E6-B098-DDCA9ED8AF3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8EB02DBB-B152-41AD-9533-88013EE04A21}"/>
   </bookViews>
@@ -38,19 +38,19 @@
     <author>HorusPC</author>
   </authors>
   <commentList>
-    <comment ref="M48" authorId="0" shapeId="0" xr:uid="{762ED5EC-C72C-4A18-A897-FD66AE10642D}">
+    <comment ref="M46" authorId="0" shapeId="0" xr:uid="{762ED5EC-C72C-4A18-A897-FD66AE10642D}">
       <text/>
     </comment>
-    <comment ref="M51" authorId="0" shapeId="0" xr:uid="{3E926ED2-AC54-4DD1-9E06-A2B266177BD9}">
+    <comment ref="M49" authorId="0" shapeId="0" xr:uid="{3E926ED2-AC54-4DD1-9E06-A2B266177BD9}">
       <text/>
     </comment>
-    <comment ref="M54" authorId="0" shapeId="0" xr:uid="{0B0F310E-15BC-40C0-BF0E-5ED516A21967}">
+    <comment ref="M52" authorId="0" shapeId="0" xr:uid="{0B0F310E-15BC-40C0-BF0E-5ED516A21967}">
       <text/>
     </comment>
-    <comment ref="M57" authorId="0" shapeId="0" xr:uid="{28FC0ADB-A958-48F2-930D-9AA4E5F0E5BF}">
+    <comment ref="M55" authorId="0" shapeId="0" xr:uid="{28FC0ADB-A958-48F2-930D-9AA4E5F0E5BF}">
       <text/>
     </comment>
-    <comment ref="M60" authorId="0" shapeId="0" xr:uid="{F2504DD1-B37A-402F-B3D8-DA8C028C09CD}">
+    <comment ref="M58" authorId="0" shapeId="0" xr:uid="{F2504DD1-B37A-402F-B3D8-DA8C028C09CD}">
       <text/>
     </comment>
   </commentList>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="125">
   <si>
     <t>productos</t>
   </si>
@@ -210,12 +210,6 @@
     <t>GIRASOL</t>
   </si>
   <si>
-    <t>pr</t>
-  </si>
-  <si>
-    <t>pr=posición relativa</t>
-  </si>
-  <si>
     <t>nombre</t>
   </si>
   <si>
@@ -249,18 +243,9 @@
     <t>BAJO ZARANDA</t>
   </si>
   <si>
-    <t>GRANOS VERDES</t>
-  </si>
-  <si>
     <t>COD PROD</t>
   </si>
   <si>
-    <t>CONTENIDO MATERIA GRASA</t>
-  </si>
-  <si>
-    <t>PUNTA NEGRA CARBON</t>
-  </si>
-  <si>
     <t>SILOS.DAT</t>
   </si>
   <si>
@@ -433,6 +418,21 @@
   </si>
   <si>
     <t>Max</t>
+  </si>
+  <si>
+    <t>autoincrem.</t>
+  </si>
+  <si>
+    <t>Cod Rub</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>A/B</t>
+  </si>
+  <si>
+    <t>P/A/C/R/F</t>
   </si>
 </sst>
 </file>
@@ -482,7 +482,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -683,11 +683,91 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -757,6 +837,61 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -830,15 +965,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -852,9 +987,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="8181975" y="3609975"/>
-          <a:ext cx="2114550" cy="1238250"/>
+        <a:xfrm>
+          <a:off x="8677275" y="3448050"/>
+          <a:ext cx="4048125" cy="1266825"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -882,16 +1017,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>695325</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>410099</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>181329</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>371999</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>133704</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -914,7 +1049,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13487400" y="6286500"/>
+          <a:off x="3124200" y="7000875"/>
           <a:ext cx="3753374" cy="2534004"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -924,6 +1059,336 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Conector recto de flecha 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8857348-3AC8-73C7-B8BD-3137EA4C5162}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8610600" y="6238875"/>
+          <a:ext cx="2952750" cy="2581275"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="Conector recto de flecha 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14AE1A1A-6150-EA4F-408D-086FC6AC65B8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8353425" y="3409950"/>
+          <a:ext cx="2619375" cy="5400675"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="26" name="Conector recto de flecha 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C892EBA-8C48-7B4C-56AC-75F16B7ED500}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13125450" y="4733925"/>
+          <a:ext cx="1809750" cy="2486025"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="28" name="Conector recto de flecha 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7F1F125-D146-42E7-5DEA-7EA48A2EFE6D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15240000" y="4610100"/>
+          <a:ext cx="523875" cy="2657475"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="30" name="Conector recto de flecha 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DAD0787-4FF8-D80C-FE99-A4C1B966B166}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="15868650" y="4572000"/>
+          <a:ext cx="85725" cy="2695575"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>171061</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2038350" cy="436786"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="32" name="CuadroTexto 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{365E06B3-E65D-B27C-8703-6357C8972A0A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15640050" y="7286236"/>
+          <a:ext cx="2038350" cy="436786"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100"/>
+            <a:t>Diferencia</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-AR" sz="1100" baseline="0"/>
+            <a:t> entre Bruto y Tara, se acumula en stock</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1224,18 +1689,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F70E36C0-A77A-46FF-BE02-DF3DE3726FE3}">
-  <dimension ref="A1:R88"/>
+  <dimension ref="A1:U88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E17" workbookViewId="0">
-      <selection activeCell="I88" sqref="H41:I88"/>
+    <sheetView tabSelected="1" topLeftCell="E16" workbookViewId="0">
+      <selection activeCell="Z22" sqref="Z22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.5703125" customWidth="1"/>
     <col min="7" max="7" width="4" customWidth="1"/>
-    <col min="12" max="12" width="2.7109375" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" customWidth="1"/>
     <col min="13" max="13" width="26.42578125" customWidth="1"/>
+    <col min="15" max="15" width="6.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
@@ -1610,11 +2076,8 @@
         <v>1</v>
       </c>
       <c r="K16" s="33"/>
-      <c r="N16" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
         <v>20</v>
       </c>
@@ -1640,15 +2103,15 @@
         <v>30</v>
       </c>
       <c r="K17" s="33"/>
-      <c r="L17" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="M17" s="8" t="s">
+      <c r="L17" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="M17" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="N17" s="8"/>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N17" s="41"/>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>0</v>
       </c>
@@ -1662,15 +2125,17 @@
       <c r="I18" s="22"/>
       <c r="J18" s="23"/>
       <c r="K18" s="33"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="N18" s="4" t="s">
+      <c r="L18" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="M18" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="N18" s="43" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>1</v>
       </c>
@@ -1684,14 +2149,17 @@
       <c r="I19" s="24"/>
       <c r="J19" s="25"/>
       <c r="K19" s="33"/>
-      <c r="L19">
-        <v>0</v>
-      </c>
-      <c r="M19" t="s">
+      <c r="L19" s="50">
+        <v>1</v>
+      </c>
+      <c r="M19" s="37" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="20" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N19" s="54" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="8">
         <v>2</v>
       </c>
@@ -1705,32 +2173,41 @@
       <c r="I20" s="26"/>
       <c r="J20" s="27"/>
       <c r="K20" s="33"/>
-      <c r="L20">
-        <v>1</v>
-      </c>
-      <c r="M20" t="s">
+      <c r="L20" s="50">
+        <v>2</v>
+      </c>
+      <c r="M20" s="37" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N20" s="54" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="K21" s="33"/>
-      <c r="L21">
-        <v>2</v>
-      </c>
-      <c r="M21" t="s">
+      <c r="L21" s="50">
+        <v>3</v>
+      </c>
+      <c r="M21" s="37" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N21" s="54" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="K22" s="33"/>
-      <c r="L22">
-        <v>3</v>
-      </c>
-      <c r="M22" t="s">
+      <c r="L22" s="50">
+        <v>4</v>
+      </c>
+      <c r="M22" s="37" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N22" s="54" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -1738,20 +2215,49 @@
         <v>36</v>
       </c>
       <c r="K23" s="33"/>
-      <c r="L23">
-        <v>4</v>
-      </c>
-      <c r="M23" t="s">
+      <c r="L23" s="51">
+        <v>5</v>
+      </c>
+      <c r="M23" s="38" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="24" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N23" s="55" t="s">
+        <v>123</v>
+      </c>
+      <c r="P23" s="60" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q23" s="61"/>
+      <c r="R23" s="61"/>
+      <c r="S23" s="61"/>
+      <c r="T23" s="61"/>
+      <c r="U23" s="62"/>
+    </row>
+    <row r="24" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
         <v>20</v>
       </c>
       <c r="K24" s="33"/>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P24" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q24" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="R24" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="S24" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="T24" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="U24" s="43" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <v>0</v>
       </c>
@@ -1759,19 +2265,18 @@
         <v>16</v>
       </c>
       <c r="K25" s="33"/>
-      <c r="L25" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="M25" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="N25" s="8"/>
-      <c r="O25" s="8"/>
-      <c r="P25" s="8"/>
-      <c r="Q25" s="8"/>
-      <c r="R25" s="8"/>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P25" s="44"/>
+      <c r="Q25" s="52">
+        <v>1</v>
+      </c>
+      <c r="R25" s="37"/>
+      <c r="S25" s="37" t="s">
+        <v>124</v>
+      </c>
+      <c r="T25" s="37"/>
+      <c r="U25" s="45"/>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
         <v>1</v>
       </c>
@@ -1779,27 +2284,18 @@
         <v>18</v>
       </c>
       <c r="K26" s="33"/>
-      <c r="L26" s="4"/>
-      <c r="M26" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="N26" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="O26" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="P26" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q26" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="R26" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P26" s="44"/>
+      <c r="Q26" s="52">
+        <v>1</v>
+      </c>
+      <c r="R26" s="37"/>
+      <c r="S26" s="37" t="s">
+        <v>124</v>
+      </c>
+      <c r="T26" s="37"/>
+      <c r="U26" s="45"/>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
         <v>2</v>
       </c>
@@ -1807,11 +2303,18 @@
         <v>17</v>
       </c>
       <c r="K27" s="33"/>
-      <c r="L27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P27" s="44"/>
+      <c r="Q27" s="52">
+        <v>5</v>
+      </c>
+      <c r="R27" s="37"/>
+      <c r="S27" s="37" t="s">
+        <v>124</v>
+      </c>
+      <c r="T27" s="37"/>
+      <c r="U27" s="45"/>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
         <v>3</v>
       </c>
@@ -1819,11 +2322,16 @@
         <v>34</v>
       </c>
       <c r="K28" s="33"/>
-      <c r="L28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P28" s="46"/>
+      <c r="Q28" s="53"/>
+      <c r="R28" s="38"/>
+      <c r="S28" s="38" t="s">
+        <v>124</v>
+      </c>
+      <c r="T28" s="38"/>
+      <c r="U28" s="47"/>
+    </row>
+    <row r="29" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="8">
         <v>4</v>
       </c>
@@ -1831,147 +2339,197 @@
         <v>35</v>
       </c>
       <c r="K29" s="33"/>
-      <c r="L29">
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="K30" s="33"/>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="K31" s="33"/>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="K32" s="33"/>
+      <c r="L32" s="39"/>
+      <c r="M32" s="41" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="33" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="K33" s="33"/>
+      <c r="L33" s="42" t="s">
+        <v>121</v>
+      </c>
+      <c r="M33" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="N33" s="34" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="K34" s="33"/>
+      <c r="L34" s="50">
+        <v>0</v>
+      </c>
+      <c r="M34" s="45" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="35" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="K35" s="33"/>
+      <c r="L35" s="50">
+        <v>1</v>
+      </c>
+      <c r="M35" s="45" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="K36" s="33"/>
+      <c r="L36" s="50">
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="K30" s="33"/>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="K31" s="33"/>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="K32" s="33"/>
-      <c r="L32" s="8"/>
-      <c r="M32" s="8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="33" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="K33" s="33"/>
-      <c r="L33" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="M33" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="N33" s="34" t="s">
+      <c r="M36" s="45" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q36" s="39"/>
+      <c r="R36" s="40" t="s">
+        <v>62</v>
+      </c>
+      <c r="S36" s="40"/>
+      <c r="T36" s="40"/>
+      <c r="U36" s="41"/>
+    </row>
+    <row r="37" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="K37" s="33"/>
+      <c r="L37" s="50">
+        <v>3</v>
+      </c>
+      <c r="M37" s="45" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q37" s="42"/>
+      <c r="R37" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="S37" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="T37" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="U37" s="43" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="38" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="K38" s="33"/>
+      <c r="L38" s="50" t="s">
+        <v>122</v>
+      </c>
+      <c r="M38" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q38" s="44"/>
+      <c r="R38" s="52">
+        <v>0</v>
+      </c>
+      <c r="S38" s="37"/>
+      <c r="T38" s="52">
+        <v>1</v>
+      </c>
+      <c r="U38" s="45"/>
+    </row>
+    <row r="39" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="K39" s="33"/>
+      <c r="L39" s="50" t="s">
+        <v>122</v>
+      </c>
+      <c r="M39" s="45" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q39" s="44"/>
+      <c r="R39" s="52">
+        <v>1</v>
+      </c>
+      <c r="S39" s="37"/>
+      <c r="T39" s="52">
+        <v>5</v>
+      </c>
+      <c r="U39" s="45"/>
+    </row>
+    <row r="40" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="K40" s="33"/>
+      <c r="L40" s="50" t="s">
+        <v>122</v>
+      </c>
+      <c r="M40" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q40" s="44"/>
+      <c r="R40" s="52">
+        <v>2</v>
+      </c>
+      <c r="S40" s="37"/>
+      <c r="T40" s="52">
+        <v>4</v>
+      </c>
+      <c r="U40" s="45"/>
+    </row>
+    <row r="41" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="H41" t="s">
+        <v>82</v>
+      </c>
+      <c r="K41" s="33"/>
+      <c r="L41" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="M41" s="47" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q41" s="44"/>
+      <c r="R41" s="52">
+        <v>3</v>
+      </c>
+      <c r="S41" s="37"/>
+      <c r="T41" s="52">
+        <v>2</v>
+      </c>
+      <c r="U41" s="45"/>
+    </row>
+    <row r="42" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="E42" t="s">
+        <v>72</v>
+      </c>
+      <c r="F42" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="34" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="K34" s="33"/>
-      <c r="L34">
-        <v>0</v>
-      </c>
-      <c r="M34" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="35" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="K35" s="33"/>
-      <c r="L35">
-        <v>1</v>
-      </c>
-      <c r="M35" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="36" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="K36" s="33"/>
-      <c r="L36">
-        <v>2</v>
-      </c>
-      <c r="M36" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="37" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="K37" s="33"/>
-      <c r="L37">
-        <v>3</v>
-      </c>
-      <c r="M37" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="38" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="K38" s="33"/>
-      <c r="L38">
-        <v>4</v>
-      </c>
-      <c r="M38" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="39" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="K39" s="33"/>
-      <c r="L39">
-        <v>5</v>
-      </c>
-      <c r="M39" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="40" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="K40" s="33"/>
-      <c r="L40">
-        <v>6</v>
-      </c>
-      <c r="M40" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="41" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="H41" t="s">
-        <v>87</v>
-      </c>
-      <c r="K41" s="33"/>
-      <c r="L41">
-        <v>7</v>
-      </c>
-      <c r="M41" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="42" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="E42" t="s">
-        <v>77</v>
-      </c>
-      <c r="F42" t="s">
-        <v>76</v>
-      </c>
       <c r="H42" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="K42" s="33"/>
-      <c r="L42">
-        <v>8</v>
-      </c>
-      <c r="M42" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="43" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="Q42" s="46"/>
+      <c r="R42" s="53" t="s">
+        <v>67</v>
+      </c>
+      <c r="S42" s="38"/>
+      <c r="T42" s="53">
+        <v>10</v>
+      </c>
+      <c r="U42" s="47"/>
+    </row>
+    <row r="43" spans="4:21" x14ac:dyDescent="0.25">
       <c r="E43" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="F43">
         <v>45</v>
       </c>
       <c r="H43" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="K43" s="33"/>
-      <c r="L43">
-        <v>9</v>
-      </c>
-      <c r="M43" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="44" spans="4:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="4:21" x14ac:dyDescent="0.25">
       <c r="E44" t="s">
         <v>6</v>
       </c>
@@ -1979,19 +2537,21 @@
         <v>30</v>
       </c>
       <c r="H44" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="K44" s="33"/>
-      <c r="L44">
-        <v>10</v>
-      </c>
-      <c r="M44" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="45" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="L44" s="56"/>
+      <c r="M44" s="56"/>
+      <c r="N44" s="57" t="s">
+        <v>52</v>
+      </c>
+      <c r="O44" s="58"/>
+      <c r="P44" s="58"/>
+      <c r="Q44" s="59"/>
+    </row>
+    <row r="45" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D45" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E45">
         <v>8</v>
@@ -2000,451 +2560,377 @@
         <v>15</v>
       </c>
       <c r="K45" s="33"/>
-    </row>
-    <row r="46" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="L45" s="56"/>
+      <c r="M45" s="56"/>
+      <c r="N45" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="O45" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="P45" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q45" s="43" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="46" spans="4:21" x14ac:dyDescent="0.25">
       <c r="E46" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="H46" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="K46" s="33"/>
-      <c r="L46" s="8"/>
-      <c r="M46" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="N46" s="8"/>
-      <c r="O46" s="8"/>
-      <c r="P46" s="8"/>
-      <c r="Q46" s="8"/>
-    </row>
-    <row r="47" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="M46" t="s">
+        <v>45</v>
+      </c>
+      <c r="N46" s="48">
+        <v>1</v>
+      </c>
+      <c r="O46" s="52">
+        <v>1</v>
+      </c>
+      <c r="P46" s="37"/>
+      <c r="Q46" s="45"/>
+    </row>
+    <row r="47" spans="4:21" x14ac:dyDescent="0.25">
       <c r="E47" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F47">
         <v>10.5</v>
       </c>
       <c r="H47" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="K47" s="33"/>
-      <c r="L47" s="4"/>
-      <c r="M47" s="4"/>
-      <c r="N47" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="O47" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="P47" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q47" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="48" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="N47" s="48">
+        <v>1</v>
+      </c>
+      <c r="O47" s="52">
+        <v>2</v>
+      </c>
+      <c r="P47" s="37"/>
+      <c r="Q47" s="45"/>
+    </row>
+    <row r="48" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D48" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E48" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F48">
         <v>18</v>
       </c>
       <c r="H48" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="K48" s="33"/>
-      <c r="L48">
+      <c r="N48" s="48">
         <v>1</v>
       </c>
-      <c r="M48" t="s">
-        <v>45</v>
-      </c>
-      <c r="N48">
-        <v>1</v>
-      </c>
-      <c r="O48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="O48" s="52">
+        <v>4</v>
+      </c>
+      <c r="P48" s="37"/>
+      <c r="Q48" s="45"/>
+    </row>
+    <row r="49" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E49" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F49">
         <v>25</v>
       </c>
       <c r="K49" s="33"/>
-      <c r="L49">
+      <c r="M49" t="s">
+        <v>46</v>
+      </c>
+      <c r="N49" s="48">
+        <v>2</v>
+      </c>
+      <c r="O49" s="52">
         <v>1</v>
       </c>
-      <c r="N49">
-        <v>1</v>
-      </c>
-      <c r="O49">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="P49" s="37"/>
+      <c r="Q49" s="45"/>
+    </row>
+    <row r="50" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D50" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E50" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F50">
         <v>6</v>
       </c>
       <c r="H50" t="s">
+        <v>89</v>
+      </c>
+      <c r="K50" s="33"/>
+      <c r="N50" s="48">
+        <v>2</v>
+      </c>
+      <c r="O50" s="52">
+        <v>4</v>
+      </c>
+      <c r="P50" s="37"/>
+      <c r="Q50" s="45"/>
+    </row>
+    <row r="51" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="H51" t="s">
+        <v>90</v>
+      </c>
+      <c r="K51" s="33"/>
+      <c r="N51" s="48">
+        <v>2</v>
+      </c>
+      <c r="O51" s="52">
+        <v>5</v>
+      </c>
+      <c r="P51" s="37"/>
+      <c r="Q51" s="45"/>
+    </row>
+    <row r="52" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="H52" t="s">
+        <v>91</v>
+      </c>
+      <c r="K52" s="33"/>
+      <c r="M52" t="s">
+        <v>47</v>
+      </c>
+      <c r="N52" s="48">
+        <v>3</v>
+      </c>
+      <c r="O52" s="52">
+        <v>1</v>
+      </c>
+      <c r="P52" s="37"/>
+      <c r="Q52" s="45"/>
+    </row>
+    <row r="53" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="H53" t="s">
+        <v>92</v>
+      </c>
+      <c r="K53" s="33"/>
+      <c r="N53" s="48">
+        <v>3</v>
+      </c>
+      <c r="O53" s="52">
+        <v>5</v>
+      </c>
+      <c r="P53" s="37"/>
+      <c r="Q53" s="45"/>
+    </row>
+    <row r="54" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="K54" s="33"/>
+      <c r="N54" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="O54" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="P54" s="37"/>
+      <c r="Q54" s="45"/>
+    </row>
+    <row r="55" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="H55" t="s">
+        <v>93</v>
+      </c>
+      <c r="K55" s="33"/>
+      <c r="M55" t="s">
+        <v>48</v>
+      </c>
+      <c r="N55" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="O55" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="P55" s="37"/>
+      <c r="Q55" s="45"/>
+    </row>
+    <row r="56" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="H56" t="s">
         <v>94</v>
       </c>
-      <c r="K50" s="33"/>
-      <c r="L50">
-        <v>1</v>
-      </c>
-      <c r="N50">
-        <v>1</v>
-      </c>
-      <c r="O50">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="51" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="H51" t="s">
+      <c r="K56" s="33"/>
+      <c r="N56" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="O56" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="P56" s="37"/>
+      <c r="Q56" s="45"/>
+    </row>
+    <row r="57" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="H57" t="s">
         <v>95</v>
       </c>
-      <c r="K51" s="33"/>
-      <c r="L51">
-        <v>2</v>
-      </c>
-      <c r="M51" t="s">
-        <v>46</v>
-      </c>
-      <c r="N51">
-        <v>2</v>
-      </c>
-      <c r="O51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="H52" t="s">
+      <c r="K57" s="33"/>
+      <c r="N57" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="O57" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="P57" s="37"/>
+      <c r="Q57" s="45"/>
+    </row>
+    <row r="58" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="H58" t="s">
         <v>96</v>
       </c>
-      <c r="K52" s="33"/>
-      <c r="L52">
-        <v>2</v>
-      </c>
-      <c r="N52">
-        <v>2</v>
-      </c>
-      <c r="O52">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="53" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="H53" t="s">
+      <c r="K58" s="33"/>
+      <c r="M58" t="s">
+        <v>49</v>
+      </c>
+      <c r="N58" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="O58" s="53" t="s">
+        <v>67</v>
+      </c>
+      <c r="P58" s="38"/>
+      <c r="Q58" s="47"/>
+    </row>
+    <row r="59" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="K59" s="33"/>
+    </row>
+    <row r="60" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="H60" t="s">
         <v>97</v>
       </c>
-      <c r="K53" s="33"/>
-      <c r="L53">
-        <v>2</v>
-      </c>
-      <c r="N53">
-        <v>2</v>
-      </c>
-      <c r="O53">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="54" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="K54" s="33"/>
-      <c r="L54">
-        <v>3</v>
-      </c>
-      <c r="M54" t="s">
-        <v>47</v>
-      </c>
-      <c r="N54">
-        <v>3</v>
-      </c>
-      <c r="O54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="H55" t="s">
+      <c r="K60" s="33"/>
+    </row>
+    <row r="61" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="H61" t="s">
         <v>98</v>
       </c>
-      <c r="K55" s="33"/>
-      <c r="L55">
-        <v>3</v>
-      </c>
-      <c r="N55">
-        <v>3</v>
-      </c>
-      <c r="O55">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="56" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="H56" t="s">
+      <c r="K61" s="33"/>
+    </row>
+    <row r="62" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="H62" t="s">
         <v>99</v>
       </c>
-      <c r="K56" s="33"/>
-      <c r="L56">
-        <v>3</v>
-      </c>
-      <c r="N56">
-        <v>3</v>
-      </c>
-      <c r="O56">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="57" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="H57" t="s">
+      <c r="K62" s="33"/>
+    </row>
+    <row r="63" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="H63" t="s">
         <v>100</v>
       </c>
-      <c r="K57" s="33"/>
-      <c r="L57">
-        <v>4</v>
-      </c>
-      <c r="M57" t="s">
-        <v>48</v>
-      </c>
-      <c r="N57">
-        <v>4</v>
-      </c>
-      <c r="O57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="H58" t="s">
+      <c r="K63" s="33"/>
+    </row>
+    <row r="64" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="K64" s="33"/>
+    </row>
+    <row r="65" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H65" t="s">
         <v>101</v>
       </c>
-      <c r="K58" s="33"/>
-      <c r="L58">
-        <v>4</v>
-      </c>
-      <c r="N58">
-        <v>4</v>
-      </c>
-      <c r="O58">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="59" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="K59" s="33"/>
-      <c r="L59">
-        <v>4</v>
-      </c>
-      <c r="N59">
-        <v>4</v>
-      </c>
-      <c r="O59">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="60" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="H60" t="s">
+      <c r="K65" s="33"/>
+    </row>
+    <row r="66" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H66" t="s">
         <v>102</v>
       </c>
-      <c r="K60" s="33"/>
-      <c r="L60">
-        <v>5</v>
-      </c>
-      <c r="M60" t="s">
-        <v>49</v>
-      </c>
-      <c r="N60">
-        <v>5</v>
-      </c>
-      <c r="O60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="H61" t="s">
+      <c r="K66" s="33"/>
+    </row>
+    <row r="67" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H67" t="s">
         <v>103</v>
       </c>
-      <c r="K61" s="33"/>
-      <c r="L61">
-        <v>5</v>
-      </c>
-      <c r="N61">
-        <v>5</v>
-      </c>
-      <c r="O61">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="62" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="H62" t="s">
+      <c r="K67" s="33"/>
+    </row>
+    <row r="68" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H68" t="s">
         <v>104</v>
       </c>
-      <c r="K62" s="33"/>
-      <c r="L62">
-        <v>5</v>
-      </c>
-      <c r="N62">
-        <v>5</v>
-      </c>
-      <c r="O62">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="63" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="H63" t="s">
+      <c r="K68" s="33"/>
+    </row>
+    <row r="69" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="K69" s="33"/>
+    </row>
+    <row r="70" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H70" t="s">
         <v>105</v>
       </c>
-      <c r="K63" s="33"/>
-    </row>
-    <row r="64" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="K64" s="33"/>
-      <c r="L64" s="8"/>
-      <c r="M64" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="N64" s="8"/>
-      <c r="O64" s="8"/>
-      <c r="P64" s="8"/>
-    </row>
-    <row r="65" spans="8:16" x14ac:dyDescent="0.25">
-      <c r="H65" t="s">
+      <c r="K70" s="33"/>
+    </row>
+    <row r="71" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H71" t="s">
         <v>106</v>
       </c>
-      <c r="K65" s="33"/>
-      <c r="L65" s="4"/>
-      <c r="M65" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="N65" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="O65" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="P65" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="66" spans="8:16" x14ac:dyDescent="0.25">
-      <c r="H66" t="s">
+      <c r="K71" s="33"/>
+    </row>
+    <row r="72" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H72" t="s">
         <v>107</v>
       </c>
-      <c r="K66" s="33"/>
-      <c r="L66">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="8:16" x14ac:dyDescent="0.25">
-      <c r="H67" t="s">
+    </row>
+    <row r="73" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H73" t="s">
         <v>108</v>
       </c>
-      <c r="K67" s="33"/>
-      <c r="L67">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="8:16" x14ac:dyDescent="0.25">
-      <c r="H68" t="s">
+    </row>
+    <row r="75" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H75" t="s">
         <v>109</v>
       </c>
-      <c r="K68" s="33"/>
-      <c r="L68">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="69" spans="8:16" x14ac:dyDescent="0.25">
-      <c r="K69" s="33"/>
-      <c r="L69">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="70" spans="8:16" x14ac:dyDescent="0.25">
-      <c r="H70" t="s">
+    </row>
+    <row r="76" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H76" t="s">
         <v>110</v>
       </c>
-      <c r="K70" s="33"/>
-      <c r="L70" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="71" spans="8:16" x14ac:dyDescent="0.25">
-      <c r="H71" t="s">
+    </row>
+    <row r="77" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H77" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="78" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H78" t="s">
         <v>111</v>
       </c>
-      <c r="K71" s="33"/>
-    </row>
-    <row r="72" spans="8:16" x14ac:dyDescent="0.25">
-      <c r="H72" t="s">
+    </row>
+    <row r="80" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H80" t="s">
         <v>112</v>
-      </c>
-    </row>
-    <row r="73" spans="8:16" x14ac:dyDescent="0.25">
-      <c r="H73" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="75" spans="8:16" x14ac:dyDescent="0.25">
-      <c r="H75" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="76" spans="8:16" x14ac:dyDescent="0.25">
-      <c r="H76" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="77" spans="8:16" x14ac:dyDescent="0.25">
-      <c r="H77" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="78" spans="8:16" x14ac:dyDescent="0.25">
-      <c r="H78" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="80" spans="8:16" x14ac:dyDescent="0.25">
-      <c r="H80" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="81" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H81" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="82" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H82" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="83" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H83" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="85" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H85" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="86" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H86" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="87" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H87" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="I87">
         <v>15</v>
@@ -2452,16 +2938,18 @@
     </row>
     <row r="88" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H88" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="I88">
         <v>30</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="D3:F3"/>
     <mergeCell ref="I3:K3"/>
+    <mergeCell ref="N44:Q44"/>
+    <mergeCell ref="P23:U23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Arregladas otras cosas y Reporte 3.
</commit_message>
<xml_diff>
--- a/datos TP3.xlsx
+++ b/datos TP3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HorusPC\Desktop\GIT-Test\tpn3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AFAAB51-C3B4-46E6-B098-DDCA9ED8AF3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39EC59BF-CA78-43D9-BA4A-33245D711976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8EB02DBB-B152-41AD-9533-88013EE04A21}"/>
   </bookViews>
@@ -835,9 +835,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
@@ -875,6 +872,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1701,7 +1701,7 @@
     <col min="7" max="7" width="4" customWidth="1"/>
     <col min="12" max="12" width="11.85546875" customWidth="1"/>
     <col min="13" max="13" width="26.42578125" customWidth="1"/>
-    <col min="15" max="15" width="6.140625" customWidth="1"/>
+    <col min="15" max="15" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
@@ -1746,17 +1746,17 @@
       <c r="B3" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
       <c r="G3" s="2"/>
-      <c r="I3" s="35" t="s">
+      <c r="I3" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="56"/>
     </row>
     <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
@@ -2103,13 +2103,13 @@
         <v>30</v>
       </c>
       <c r="K17" s="33"/>
-      <c r="L17" s="39" t="s">
+      <c r="L17" s="38" t="s">
         <v>120</v>
       </c>
-      <c r="M17" s="40" t="s">
+      <c r="M17" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="N17" s="41"/>
+      <c r="N17" s="40"/>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
@@ -2125,13 +2125,13 @@
       <c r="I18" s="22"/>
       <c r="J18" s="23"/>
       <c r="K18" s="33"/>
-      <c r="L18" s="42" t="s">
+      <c r="L18" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="M18" s="36" t="s">
+      <c r="M18" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="N18" s="43" t="s">
+      <c r="N18" s="42" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2149,13 +2149,13 @@
       <c r="I19" s="24"/>
       <c r="J19" s="25"/>
       <c r="K19" s="33"/>
-      <c r="L19" s="50">
+      <c r="L19" s="49">
         <v>1</v>
       </c>
-      <c r="M19" s="37" t="s">
+      <c r="M19" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="N19" s="54" t="s">
+      <c r="N19" s="53" t="s">
         <v>123</v>
       </c>
     </row>
@@ -2173,37 +2173,37 @@
       <c r="I20" s="26"/>
       <c r="J20" s="27"/>
       <c r="K20" s="33"/>
-      <c r="L20" s="50">
+      <c r="L20" s="49">
         <v>2</v>
       </c>
-      <c r="M20" s="37" t="s">
+      <c r="M20" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="N20" s="54" t="s">
+      <c r="N20" s="53" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="K21" s="33"/>
-      <c r="L21" s="50">
+      <c r="L21" s="49">
         <v>3</v>
       </c>
-      <c r="M21" s="37" t="s">
+      <c r="M21" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="N21" s="54" t="s">
+      <c r="N21" s="53" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="K22" s="33"/>
-      <c r="L22" s="50">
+      <c r="L22" s="49">
         <v>4</v>
       </c>
-      <c r="M22" s="37" t="s">
+      <c r="M22" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="N22" s="54" t="s">
+      <c r="N22" s="53" t="s">
         <v>123</v>
       </c>
     </row>
@@ -2215,13 +2215,13 @@
         <v>36</v>
       </c>
       <c r="K23" s="33"/>
-      <c r="L23" s="51">
+      <c r="L23" s="50">
         <v>5</v>
       </c>
-      <c r="M23" s="38" t="s">
+      <c r="M23" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="N23" s="55" t="s">
+      <c r="N23" s="54" t="s">
         <v>123</v>
       </c>
       <c r="P23" s="60" t="s">
@@ -2238,22 +2238,22 @@
         <v>20</v>
       </c>
       <c r="K24" s="33"/>
-      <c r="P24" s="42" t="s">
+      <c r="P24" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="Q24" s="36" t="s">
+      <c r="Q24" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="R24" s="36" t="s">
+      <c r="R24" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="S24" s="36" t="s">
+      <c r="S24" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="T24" s="36" t="s">
+      <c r="T24" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="U24" s="43" t="s">
+      <c r="U24" s="42" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2265,16 +2265,16 @@
         <v>16</v>
       </c>
       <c r="K25" s="33"/>
-      <c r="P25" s="44"/>
-      <c r="Q25" s="52">
+      <c r="P25" s="43"/>
+      <c r="Q25" s="51">
         <v>1</v>
       </c>
-      <c r="R25" s="37"/>
-      <c r="S25" s="37" t="s">
+      <c r="R25" s="36"/>
+      <c r="S25" s="36" t="s">
         <v>124</v>
       </c>
-      <c r="T25" s="37"/>
-      <c r="U25" s="45"/>
+      <c r="T25" s="36"/>
+      <c r="U25" s="44"/>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
@@ -2284,16 +2284,16 @@
         <v>18</v>
       </c>
       <c r="K26" s="33"/>
-      <c r="P26" s="44"/>
-      <c r="Q26" s="52">
+      <c r="P26" s="43"/>
+      <c r="Q26" s="51">
         <v>1</v>
       </c>
-      <c r="R26" s="37"/>
-      <c r="S26" s="37" t="s">
+      <c r="R26" s="36"/>
+      <c r="S26" s="36" t="s">
         <v>124</v>
       </c>
-      <c r="T26" s="37"/>
-      <c r="U26" s="45"/>
+      <c r="T26" s="36"/>
+      <c r="U26" s="44"/>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
@@ -2303,16 +2303,16 @@
         <v>17</v>
       </c>
       <c r="K27" s="33"/>
-      <c r="P27" s="44"/>
-      <c r="Q27" s="52">
+      <c r="P27" s="43"/>
+      <c r="Q27" s="51">
         <v>5</v>
       </c>
-      <c r="R27" s="37"/>
-      <c r="S27" s="37" t="s">
+      <c r="R27" s="36"/>
+      <c r="S27" s="36" t="s">
         <v>124</v>
       </c>
-      <c r="T27" s="37"/>
-      <c r="U27" s="45"/>
+      <c r="T27" s="36"/>
+      <c r="U27" s="44"/>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
@@ -2322,14 +2322,14 @@
         <v>34</v>
       </c>
       <c r="K28" s="33"/>
-      <c r="P28" s="46"/>
-      <c r="Q28" s="53"/>
-      <c r="R28" s="38"/>
-      <c r="S28" s="38" t="s">
+      <c r="P28" s="45"/>
+      <c r="Q28" s="52"/>
+      <c r="R28" s="37"/>
+      <c r="S28" s="37" t="s">
         <v>124</v>
       </c>
-      <c r="T28" s="38"/>
-      <c r="U28" s="47"/>
+      <c r="T28" s="37"/>
+      <c r="U28" s="46"/>
     </row>
     <row r="29" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="8">
@@ -2348,17 +2348,17 @@
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="K32" s="33"/>
-      <c r="L32" s="39"/>
-      <c r="M32" s="41" t="s">
+      <c r="L32" s="38"/>
+      <c r="M32" s="40" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="33" spans="4:21" x14ac:dyDescent="0.25">
       <c r="K33" s="33"/>
-      <c r="L33" s="42" t="s">
+      <c r="L33" s="41" t="s">
         <v>121</v>
       </c>
-      <c r="M33" s="43" t="s">
+      <c r="M33" s="42" t="s">
         <v>50</v>
       </c>
       <c r="N33" s="34" t="s">
@@ -2367,134 +2367,134 @@
     </row>
     <row r="34" spans="4:21" x14ac:dyDescent="0.25">
       <c r="K34" s="33"/>
-      <c r="L34" s="50">
+      <c r="L34" s="49">
         <v>0</v>
       </c>
-      <c r="M34" s="45" t="s">
+      <c r="M34" s="44" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="35" spans="4:21" x14ac:dyDescent="0.25">
       <c r="K35" s="33"/>
-      <c r="L35" s="50">
+      <c r="L35" s="49">
         <v>1</v>
       </c>
-      <c r="M35" s="45" t="s">
+      <c r="M35" s="44" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="36" spans="4:21" x14ac:dyDescent="0.25">
       <c r="K36" s="33"/>
-      <c r="L36" s="50">
+      <c r="L36" s="49">
         <v>2</v>
       </c>
-      <c r="M36" s="45" t="s">
+      <c r="M36" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="Q36" s="39"/>
-      <c r="R36" s="40" t="s">
+      <c r="Q36" s="38"/>
+      <c r="R36" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="S36" s="40"/>
-      <c r="T36" s="40"/>
-      <c r="U36" s="41"/>
+      <c r="S36" s="39"/>
+      <c r="T36" s="39"/>
+      <c r="U36" s="40"/>
     </row>
     <row r="37" spans="4:21" x14ac:dyDescent="0.25">
       <c r="K37" s="33"/>
-      <c r="L37" s="50">
+      <c r="L37" s="49">
         <v>3</v>
       </c>
-      <c r="M37" s="45" t="s">
+      <c r="M37" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="Q37" s="42"/>
-      <c r="R37" s="36" t="s">
+      <c r="Q37" s="41"/>
+      <c r="R37" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="S37" s="36" t="s">
+      <c r="S37" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="T37" s="36" t="s">
+      <c r="T37" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="U37" s="43" t="s">
+      <c r="U37" s="42" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="38" spans="4:21" x14ac:dyDescent="0.25">
       <c r="K38" s="33"/>
-      <c r="L38" s="50" t="s">
+      <c r="L38" s="49" t="s">
         <v>122</v>
       </c>
-      <c r="M38" s="45" t="s">
+      <c r="M38" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="Q38" s="44"/>
-      <c r="R38" s="52">
+      <c r="Q38" s="43"/>
+      <c r="R38" s="51">
         <v>0</v>
       </c>
-      <c r="S38" s="37"/>
-      <c r="T38" s="52">
+      <c r="S38" s="36"/>
+      <c r="T38" s="51">
         <v>1</v>
       </c>
-      <c r="U38" s="45"/>
+      <c r="U38" s="44"/>
     </row>
     <row r="39" spans="4:21" x14ac:dyDescent="0.25">
       <c r="K39" s="33"/>
-      <c r="L39" s="50" t="s">
+      <c r="L39" s="49" t="s">
         <v>122</v>
       </c>
-      <c r="M39" s="45" t="s">
+      <c r="M39" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="Q39" s="44"/>
-      <c r="R39" s="52">
+      <c r="Q39" s="43"/>
+      <c r="R39" s="51">
         <v>1</v>
       </c>
-      <c r="S39" s="37"/>
-      <c r="T39" s="52">
+      <c r="S39" s="36"/>
+      <c r="T39" s="51">
         <v>5</v>
       </c>
-      <c r="U39" s="45"/>
+      <c r="U39" s="44"/>
     </row>
     <row r="40" spans="4:21" x14ac:dyDescent="0.25">
       <c r="K40" s="33"/>
-      <c r="L40" s="50" t="s">
+      <c r="L40" s="49" t="s">
         <v>122</v>
       </c>
-      <c r="M40" s="45" t="s">
+      <c r="M40" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="Q40" s="44"/>
-      <c r="R40" s="52">
+      <c r="Q40" s="43"/>
+      <c r="R40" s="51">
         <v>2</v>
       </c>
-      <c r="S40" s="37"/>
-      <c r="T40" s="52">
+      <c r="S40" s="36"/>
+      <c r="T40" s="51">
         <v>4</v>
       </c>
-      <c r="U40" s="45"/>
+      <c r="U40" s="44"/>
     </row>
     <row r="41" spans="4:21" x14ac:dyDescent="0.25">
       <c r="H41" t="s">
         <v>82</v>
       </c>
       <c r="K41" s="33"/>
-      <c r="L41" s="51" t="s">
+      <c r="L41" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="M41" s="47" t="s">
+      <c r="M41" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="Q41" s="44"/>
-      <c r="R41" s="52">
+      <c r="Q41" s="43"/>
+      <c r="R41" s="51">
         <v>3</v>
       </c>
-      <c r="S41" s="37"/>
-      <c r="T41" s="52">
+      <c r="S41" s="36"/>
+      <c r="T41" s="51">
         <v>2</v>
       </c>
-      <c r="U41" s="45"/>
+      <c r="U41" s="44"/>
     </row>
     <row r="42" spans="4:21" x14ac:dyDescent="0.25">
       <c r="E42" t="s">
@@ -2507,15 +2507,15 @@
         <v>83</v>
       </c>
       <c r="K42" s="33"/>
-      <c r="Q42" s="46"/>
-      <c r="R42" s="53" t="s">
+      <c r="Q42" s="45"/>
+      <c r="R42" s="52" t="s">
         <v>67</v>
       </c>
-      <c r="S42" s="38"/>
-      <c r="T42" s="53">
+      <c r="S42" s="37"/>
+      <c r="T42" s="52">
         <v>10</v>
       </c>
-      <c r="U42" s="47"/>
+      <c r="U42" s="46"/>
     </row>
     <row r="43" spans="4:21" x14ac:dyDescent="0.25">
       <c r="E43" t="s">
@@ -2540,8 +2540,8 @@
         <v>85</v>
       </c>
       <c r="K44" s="33"/>
-      <c r="L44" s="56"/>
-      <c r="M44" s="56"/>
+      <c r="L44" s="55"/>
+      <c r="M44" s="55"/>
       <c r="N44" s="57" t="s">
         <v>52</v>
       </c>
@@ -2560,18 +2560,18 @@
         <v>15</v>
       </c>
       <c r="K45" s="33"/>
-      <c r="L45" s="56"/>
-      <c r="M45" s="56"/>
-      <c r="N45" s="42" t="s">
+      <c r="L45" s="55"/>
+      <c r="M45" s="55"/>
+      <c r="N45" s="41" t="s">
         <v>61</v>
       </c>
-      <c r="O45" s="36" t="s">
+      <c r="O45" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="P45" s="36" t="s">
+      <c r="P45" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="Q45" s="43" t="s">
+      <c r="Q45" s="42" t="s">
         <v>70</v>
       </c>
     </row>
@@ -2586,14 +2586,14 @@
       <c r="M46" t="s">
         <v>45</v>
       </c>
-      <c r="N46" s="48">
+      <c r="N46" s="47">
         <v>1</v>
       </c>
-      <c r="O46" s="52">
+      <c r="O46" s="51">
         <v>1</v>
       </c>
-      <c r="P46" s="37"/>
-      <c r="Q46" s="45"/>
+      <c r="P46" s="36"/>
+      <c r="Q46" s="44"/>
     </row>
     <row r="47" spans="4:21" x14ac:dyDescent="0.25">
       <c r="E47" t="s">
@@ -2606,14 +2606,14 @@
         <v>87</v>
       </c>
       <c r="K47" s="33"/>
-      <c r="N47" s="48">
+      <c r="N47" s="47">
         <v>1</v>
       </c>
-      <c r="O47" s="52">
+      <c r="O47" s="51">
         <v>2</v>
       </c>
-      <c r="P47" s="37"/>
-      <c r="Q47" s="45"/>
+      <c r="P47" s="36"/>
+      <c r="Q47" s="44"/>
     </row>
     <row r="48" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D48" t="s">
@@ -2629,14 +2629,14 @@
         <v>88</v>
       </c>
       <c r="K48" s="33"/>
-      <c r="N48" s="48">
+      <c r="N48" s="47">
         <v>1</v>
       </c>
-      <c r="O48" s="52">
+      <c r="O48" s="51">
         <v>4</v>
       </c>
-      <c r="P48" s="37"/>
-      <c r="Q48" s="45"/>
+      <c r="P48" s="36"/>
+      <c r="Q48" s="44"/>
     </row>
     <row r="49" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E49" t="s">
@@ -2649,14 +2649,14 @@
       <c r="M49" t="s">
         <v>46</v>
       </c>
-      <c r="N49" s="48">
+      <c r="N49" s="47">
         <v>2</v>
       </c>
-      <c r="O49" s="52">
+      <c r="O49" s="51">
         <v>1</v>
       </c>
-      <c r="P49" s="37"/>
-      <c r="Q49" s="45"/>
+      <c r="P49" s="36"/>
+      <c r="Q49" s="44"/>
     </row>
     <row r="50" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D50" t="s">
@@ -2672,28 +2672,28 @@
         <v>89</v>
       </c>
       <c r="K50" s="33"/>
-      <c r="N50" s="48">
+      <c r="N50" s="47">
         <v>2</v>
       </c>
-      <c r="O50" s="52">
+      <c r="O50" s="51">
         <v>4</v>
       </c>
-      <c r="P50" s="37"/>
-      <c r="Q50" s="45"/>
+      <c r="P50" s="36"/>
+      <c r="Q50" s="44"/>
     </row>
     <row r="51" spans="4:17" x14ac:dyDescent="0.25">
       <c r="H51" t="s">
         <v>90</v>
       </c>
       <c r="K51" s="33"/>
-      <c r="N51" s="48">
+      <c r="N51" s="47">
         <v>2</v>
       </c>
-      <c r="O51" s="52">
+      <c r="O51" s="51">
         <v>5</v>
       </c>
-      <c r="P51" s="37"/>
-      <c r="Q51" s="45"/>
+      <c r="P51" s="36"/>
+      <c r="Q51" s="44"/>
     </row>
     <row r="52" spans="4:17" x14ac:dyDescent="0.25">
       <c r="H52" t="s">
@@ -2703,39 +2703,39 @@
       <c r="M52" t="s">
         <v>47</v>
       </c>
-      <c r="N52" s="48">
+      <c r="N52" s="47">
         <v>3</v>
       </c>
-      <c r="O52" s="52">
+      <c r="O52" s="51">
         <v>1</v>
       </c>
-      <c r="P52" s="37"/>
-      <c r="Q52" s="45"/>
+      <c r="P52" s="36"/>
+      <c r="Q52" s="44"/>
     </row>
     <row r="53" spans="4:17" x14ac:dyDescent="0.25">
       <c r="H53" t="s">
         <v>92</v>
       </c>
       <c r="K53" s="33"/>
-      <c r="N53" s="48">
+      <c r="N53" s="47">
         <v>3</v>
       </c>
-      <c r="O53" s="52">
+      <c r="O53" s="51">
         <v>5</v>
       </c>
-      <c r="P53" s="37"/>
-      <c r="Q53" s="45"/>
+      <c r="P53" s="36"/>
+      <c r="Q53" s="44"/>
     </row>
     <row r="54" spans="4:17" x14ac:dyDescent="0.25">
       <c r="K54" s="33"/>
-      <c r="N54" s="48" t="s">
+      <c r="N54" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="O54" s="52" t="s">
+      <c r="O54" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="P54" s="37"/>
-      <c r="Q54" s="45"/>
+      <c r="P54" s="36"/>
+      <c r="Q54" s="44"/>
     </row>
     <row r="55" spans="4:17" x14ac:dyDescent="0.25">
       <c r="H55" t="s">
@@ -2745,42 +2745,42 @@
       <c r="M55" t="s">
         <v>48</v>
       </c>
-      <c r="N55" s="48" t="s">
+      <c r="N55" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="O55" s="52" t="s">
+      <c r="O55" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="P55" s="37"/>
-      <c r="Q55" s="45"/>
+      <c r="P55" s="36"/>
+      <c r="Q55" s="44"/>
     </row>
     <row r="56" spans="4:17" x14ac:dyDescent="0.25">
       <c r="H56" t="s">
         <v>94</v>
       </c>
       <c r="K56" s="33"/>
-      <c r="N56" s="48" t="s">
+      <c r="N56" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="O56" s="52" t="s">
+      <c r="O56" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="P56" s="37"/>
-      <c r="Q56" s="45"/>
+      <c r="P56" s="36"/>
+      <c r="Q56" s="44"/>
     </row>
     <row r="57" spans="4:17" x14ac:dyDescent="0.25">
       <c r="H57" t="s">
         <v>95</v>
       </c>
       <c r="K57" s="33"/>
-      <c r="N57" s="48" t="s">
+      <c r="N57" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="O57" s="52" t="s">
+      <c r="O57" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="P57" s="37"/>
-      <c r="Q57" s="45"/>
+      <c r="P57" s="36"/>
+      <c r="Q57" s="44"/>
     </row>
     <row r="58" spans="4:17" x14ac:dyDescent="0.25">
       <c r="H58" t="s">
@@ -2790,14 +2790,14 @@
       <c r="M58" t="s">
         <v>49</v>
       </c>
-      <c r="N58" s="49" t="s">
+      <c r="N58" s="48" t="s">
         <v>67</v>
       </c>
-      <c r="O58" s="53" t="s">
+      <c r="O58" s="52" t="s">
         <v>67</v>
       </c>
-      <c r="P58" s="38"/>
-      <c r="Q58" s="47"/>
+      <c r="P58" s="37"/>
+      <c r="Q58" s="46"/>
     </row>
     <row r="59" spans="4:17" x14ac:dyDescent="0.25">
       <c r="K59" s="33"/>

</xml_diff>

<commit_message>
Verificado bastante. Si da problemas borrar archivo operaciones.dat
</commit_message>
<xml_diff>
--- a/datos TP3.xlsx
+++ b/datos TP3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HorusPC\Desktop\GIT-Test\tpn3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39EC59BF-CA78-43D9-BA4A-33245D711976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A0F939-0997-4D21-9AFF-8047AE1844C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8EB02DBB-B152-41AD-9533-88013EE04A21}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="125">
   <si>
     <t>productos</t>
   </si>
@@ -767,7 +767,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -872,6 +872,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -891,6 +894,25 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1689,10 +1711,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F70E36C0-A77A-46FF-BE02-DF3DE3726FE3}">
-  <dimension ref="A1:U88"/>
+  <dimension ref="A1:V88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E16" workbookViewId="0">
-      <selection activeCell="Z22" sqref="Z22"/>
+    <sheetView tabSelected="1" topLeftCell="E17" workbookViewId="0">
+      <selection activeCell="X21" sqref="X21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1746,17 +1768,17 @@
       <c r="B3" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="56" t="s">
+      <c r="D3" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
       <c r="G3" s="2"/>
-      <c r="I3" s="56" t="s">
+      <c r="I3" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="56"/>
-      <c r="K3" s="56"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
     </row>
     <row r="4" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
@@ -2077,7 +2099,7 @@
       </c>
       <c r="K16" s="33"/>
     </row>
-    <row r="17" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
         <v>20</v>
       </c>
@@ -2106,12 +2128,12 @@
       <c r="L17" s="38" t="s">
         <v>120</v>
       </c>
-      <c r="M17" s="39" t="s">
+      <c r="M17" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="N17" s="40"/>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="N17" s="63"/>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>0</v>
       </c>
@@ -2135,7 +2157,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>1</v>
       </c>
@@ -2159,7 +2181,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="8">
         <v>2</v>
       </c>
@@ -2183,7 +2205,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="K21" s="33"/>
       <c r="L21" s="49">
         <v>3</v>
@@ -2195,7 +2217,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="K22" s="33"/>
       <c r="L22" s="49">
         <v>4</v>
@@ -2207,7 +2229,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -2215,8 +2237,8 @@
         <v>36</v>
       </c>
       <c r="K23" s="33"/>
-      <c r="L23" s="50">
-        <v>5</v>
+      <c r="L23" s="50" t="s">
+        <v>67</v>
       </c>
       <c r="M23" s="37" t="s">
         <v>49</v>
@@ -2224,40 +2246,44 @@
       <c r="N23" s="54" t="s">
         <v>123</v>
       </c>
-      <c r="P23" s="60" t="s">
+      <c r="P23" s="61" t="s">
         <v>37</v>
       </c>
-      <c r="Q23" s="61"/>
-      <c r="R23" s="61"/>
-      <c r="S23" s="61"/>
-      <c r="T23" s="61"/>
+      <c r="Q23" s="62"/>
+      <c r="R23" s="62"/>
+      <c r="S23" s="62"/>
+      <c r="T23" s="62"/>
       <c r="U23" s="62"/>
-    </row>
-    <row r="24" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V23" s="63"/>
+    </row>
+    <row r="24" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
         <v>20</v>
       </c>
       <c r="K24" s="33"/>
-      <c r="P24" s="41" t="s">
+      <c r="P24" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="Q24" s="35" t="s">
+      <c r="Q24" s="66" t="s">
         <v>40</v>
       </c>
-      <c r="R24" s="35" t="s">
+      <c r="R24" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="S24" s="35" t="s">
+      <c r="S24" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="T24" s="35" t="s">
+      <c r="T24" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="U24" s="42" t="s">
+      <c r="U24" s="66" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V24" s="67" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <v>0</v>
       </c>
@@ -2274,9 +2300,10 @@
         <v>124</v>
       </c>
       <c r="T25" s="36"/>
-      <c r="U25" s="44"/>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U25" s="36"/>
+      <c r="V25" s="44"/>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
         <v>1</v>
       </c>
@@ -2293,9 +2320,10 @@
         <v>124</v>
       </c>
       <c r="T26" s="36"/>
-      <c r="U26" s="44"/>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U26" s="36"/>
+      <c r="V26" s="44"/>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
         <v>2</v>
       </c>
@@ -2312,9 +2340,10 @@
         <v>124</v>
       </c>
       <c r="T27" s="36"/>
-      <c r="U27" s="44"/>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U27" s="36"/>
+      <c r="V27" s="44"/>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
         <v>3</v>
       </c>
@@ -2329,9 +2358,10 @@
         <v>124</v>
       </c>
       <c r="T28" s="37"/>
-      <c r="U28" s="46"/>
-    </row>
-    <row r="29" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U28" s="37"/>
+      <c r="V28" s="46"/>
+    </row>
+    <row r="29" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="8">
         <v>4</v>
       </c>
@@ -2340,25 +2370,27 @@
       </c>
       <c r="K29" s="33"/>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="K30" s="33"/>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="K31" s="33"/>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="K32" s="33"/>
-      <c r="L32" s="38"/>
-      <c r="M32" s="40" t="s">
+      <c r="L32" s="38" t="s">
+        <v>120</v>
+      </c>
+      <c r="M32" s="56" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="33" spans="4:21" x14ac:dyDescent="0.25">
       <c r="K33" s="33"/>
-      <c r="L33" s="41" t="s">
+      <c r="L33" s="65" t="s">
         <v>121</v>
       </c>
-      <c r="M33" s="42" t="s">
+      <c r="M33" s="67" t="s">
         <v>50</v>
       </c>
       <c r="N33" s="34" t="s">
@@ -2368,7 +2400,7 @@
     <row r="34" spans="4:21" x14ac:dyDescent="0.25">
       <c r="K34" s="33"/>
       <c r="L34" s="49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M34" s="44" t="s">
         <v>53</v>
@@ -2377,7 +2409,7 @@
     <row r="35" spans="4:21" x14ac:dyDescent="0.25">
       <c r="K35" s="33"/>
       <c r="L35" s="49">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M35" s="44" t="s">
         <v>54</v>
@@ -2386,38 +2418,40 @@
     <row r="36" spans="4:21" x14ac:dyDescent="0.25">
       <c r="K36" s="33"/>
       <c r="L36" s="49">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M36" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="Q36" s="38"/>
-      <c r="R36" s="39" t="s">
+      <c r="Q36" s="64"/>
+      <c r="R36" s="38" t="s">
+        <v>120</v>
+      </c>
+      <c r="S36" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="S36" s="39"/>
       <c r="T36" s="39"/>
       <c r="U36" s="40"/>
     </row>
     <row r="37" spans="4:21" x14ac:dyDescent="0.25">
       <c r="K37" s="33"/>
       <c r="L37" s="49">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M37" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="Q37" s="41"/>
-      <c r="R37" s="35" t="s">
+      <c r="Q37" s="64"/>
+      <c r="R37" s="70" t="s">
         <v>63</v>
       </c>
-      <c r="S37" s="35" t="s">
+      <c r="S37" s="68" t="s">
         <v>64</v>
       </c>
-      <c r="T37" s="35" t="s">
+      <c r="T37" s="68" t="s">
         <v>61</v>
       </c>
-      <c r="U37" s="42" t="s">
+      <c r="U37" s="69" t="s">
         <v>65</v>
       </c>
     </row>
@@ -2429,9 +2463,9 @@
       <c r="M38" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="Q38" s="43"/>
-      <c r="R38" s="51">
-        <v>0</v>
+      <c r="Q38" s="64"/>
+      <c r="R38" s="47">
+        <v>1</v>
       </c>
       <c r="S38" s="36"/>
       <c r="T38" s="51">
@@ -2447,9 +2481,9 @@
       <c r="M39" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="Q39" s="43"/>
-      <c r="R39" s="51">
-        <v>1</v>
+      <c r="Q39" s="64"/>
+      <c r="R39" s="47">
+        <v>2</v>
       </c>
       <c r="S39" s="36"/>
       <c r="T39" s="51">
@@ -2465,9 +2499,9 @@
       <c r="M40" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="Q40" s="43"/>
-      <c r="R40" s="51">
-        <v>2</v>
+      <c r="Q40" s="64"/>
+      <c r="R40" s="47">
+        <v>3</v>
       </c>
       <c r="S40" s="36"/>
       <c r="T40" s="51">
@@ -2486,9 +2520,9 @@
       <c r="M41" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="Q41" s="43"/>
-      <c r="R41" s="51">
-        <v>3</v>
+      <c r="Q41" s="64"/>
+      <c r="R41" s="47">
+        <v>4</v>
       </c>
       <c r="S41" s="36"/>
       <c r="T41" s="51">
@@ -2507,8 +2541,8 @@
         <v>83</v>
       </c>
       <c r="K42" s="33"/>
-      <c r="Q42" s="45"/>
-      <c r="R42" s="52" t="s">
+      <c r="Q42" s="64"/>
+      <c r="R42" s="48" t="s">
         <v>67</v>
       </c>
       <c r="S42" s="37"/>
@@ -2542,12 +2576,12 @@
       <c r="K44" s="33"/>
       <c r="L44" s="55"/>
       <c r="M44" s="55"/>
-      <c r="N44" s="57" t="s">
+      <c r="N44" s="58" t="s">
         <v>52</v>
       </c>
-      <c r="O44" s="58"/>
-      <c r="P44" s="58"/>
-      <c r="Q44" s="59"/>
+      <c r="O44" s="59"/>
+      <c r="P44" s="59"/>
+      <c r="Q44" s="60"/>
     </row>
     <row r="45" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D45" t="s">
@@ -2562,16 +2596,16 @@
       <c r="K45" s="33"/>
       <c r="L45" s="55"/>
       <c r="M45" s="55"/>
-      <c r="N45" s="41" t="s">
+      <c r="N45" s="65" t="s">
         <v>61</v>
       </c>
-      <c r="O45" s="35" t="s">
+      <c r="O45" s="66" t="s">
         <v>68</v>
       </c>
-      <c r="P45" s="35" t="s">
+      <c r="P45" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="Q45" s="42" t="s">
+      <c r="Q45" s="67" t="s">
         <v>70</v>
       </c>
     </row>
@@ -2945,11 +2979,12 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="D3:F3"/>
     <mergeCell ref="I3:K3"/>
     <mergeCell ref="N44:Q44"/>
-    <mergeCell ref="P23:U23"/>
+    <mergeCell ref="P23:V23"/>
+    <mergeCell ref="M17:N17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>